<commit_message>
feat : Documentos corregidos: costos y ficha tecnica
</commit_message>
<xml_diff>
--- a/Docs/02-DESING/04-Costos/costos_knstore-modfxlsx.xlsx
+++ b/Docs/02-DESING/04-Costos/costos_knstore-modfxlsx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11580" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen Ejecutivo" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
   <si>
     <t>Indicador</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t>Adaptación móvil, tablet, desktop</t>
+  </si>
+  <si>
+    <t>Nomina</t>
+  </si>
+  <si>
+    <t>Nomina del personal del desarrollo</t>
+  </si>
+  <si>
+    <t>El valor 328 es el resultado de la suma de horas totales</t>
   </si>
   <si>
     <t>total</t>
@@ -248,14 +257,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="&quot;$&quot;#,###.##000_);[Red]\(&quot;$&quot;#,###.##000\)"/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,###.##000_);[Red]\(&quot;$&quot;#,###.##000\)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -433,7 +441,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,12 +464,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
         <bgColor rgb="FF1F4E78"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -851,7 +853,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -875,16 +877,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -893,89 +895,89 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -986,19 +988,13 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1007,10 +1003,7 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1022,16 +1015,13 @@
     <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1040,7 +1030,7 @@
     <xf numFmtId="44" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1049,22 +1039,19 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1073,18 +1060,18 @@
     <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1094,7 +1081,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1106,9 +1093,6 @@
     <xf numFmtId="6" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1118,10 +1102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1320,7 +1301,7 @@
                 <c:formatCode>"$"#,###.##000_);[Red]\("$"#,###.##000\)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>19480000</c:v>
+                  <c:v>33400000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3130488</c:v>
@@ -1988,84 +1969,84 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="21" style="35" customWidth="1"/>
-    <col min="2" max="2" width="40" style="35" customWidth="1"/>
-    <col min="3" max="3" width="55.2857142857143" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="35"/>
+    <col min="1" max="1" width="21" style="7" customWidth="1"/>
+    <col min="2" max="2" width="40" style="7" customWidth="1"/>
+    <col min="3" max="3" width="55.2857142857143" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="48">
-        <f>SUM(CAPEX!G12)</f>
-        <v>19480000</v>
-      </c>
-      <c r="C2" s="47"/>
+      <c r="B2" s="9">
+        <f>SUM(CAPEX!G13)</f>
+        <v>33400000</v>
+      </c>
+      <c r="C2" s="41"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="9">
         <f>SUM(OPEX!E7)</f>
         <v>3130488</v>
       </c>
-      <c r="C3" s="47"/>
+      <c r="C3" s="41"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="9">
         <f>OPEX!F7</f>
         <v>9391464</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="41"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="9">
         <f>OPEX!G7</f>
         <v>15652440</v>
       </c>
-      <c r="C5" s="47"/>
+      <c r="C5" s="41"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="41">
         <f>(B2*0.15)/B4</f>
-        <v>0.311133599617695</v>
-      </c>
-      <c r="C6" s="47" t="s">
+        <v>0.533463153348615</v>
+      </c>
+      <c r="C6" s="41" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="42">
         <f>SUM(B2:B6)</f>
-        <v>47654392.3111336</v>
-      </c>
-      <c r="C7" s="49" t="s">
+        <v>61574392.5334632</v>
+      </c>
+      <c r="C7" s="42" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2078,455 +2059,488 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I125"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.4285714285714" style="17" customWidth="1"/>
-    <col min="2" max="2" width="50.2857142857143" style="17" customWidth="1"/>
-    <col min="3" max="3" width="16.2857142857143" style="17" customWidth="1"/>
-    <col min="4" max="4" width="16.2857142857143" style="18" customWidth="1"/>
-    <col min="5" max="5" width="17" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.2857142857143" style="19" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.4285714285714" style="19" customWidth="1"/>
-    <col min="8" max="8" width="16.2857142857143" style="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="50.2857142857143" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="17"/>
+    <col min="1" max="1" width="20.4285714285714" style="13" customWidth="1"/>
+    <col min="2" max="2" width="50.2857142857143" style="13" customWidth="1"/>
+    <col min="3" max="3" width="16.2857142857143" style="13" customWidth="1"/>
+    <col min="4" max="4" width="16.2857142857143" style="14" customWidth="1"/>
+    <col min="5" max="5" width="17" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.2857142857143" style="15" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.4285714285714" style="15" customWidth="1"/>
+    <col min="8" max="8" width="16.2857142857143" style="13" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="50.2857142857143" style="13" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E2" s="23">
+      <c r="D2" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E2" s="19">
         <v>30</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="21">
         <f>D2*E2</f>
-        <v>1800000</v>
-      </c>
-      <c r="G2" s="25">
-        <f>D2*E2</f>
-        <v>1800000</v>
-      </c>
-      <c r="H2" s="23" t="s">
+        <v>600000</v>
+      </c>
+      <c r="G2" s="21">
+        <f t="shared" ref="G2:G10" si="0">D2*E2</f>
+        <v>600000</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E3" s="23">
+      <c r="D3" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E3" s="19">
         <v>35</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="21">
         <v>1700000</v>
       </c>
-      <c r="G3" s="25">
-        <f>D3*E3</f>
+      <c r="G3" s="21">
+        <f t="shared" si="0"/>
+        <v>700000</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E4" s="19">
+        <v>35</v>
+      </c>
+      <c r="F4" s="21">
         <v>2100000</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="G4" s="21">
+        <f t="shared" si="0"/>
+        <v>700000</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="23"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E5" s="23">
+        <v>40</v>
+      </c>
+      <c r="F5" s="24">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24">
+        <f t="shared" si="0"/>
+        <v>800000</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E6" s="19">
+        <v>38</v>
+      </c>
+      <c r="F6" s="21">
+        <v>2086000</v>
+      </c>
+      <c r="G6" s="21">
+        <f t="shared" si="0"/>
+        <v>760000</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E7" s="19">
+        <v>45</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2000000</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="0"/>
+        <v>900000</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E8" s="19">
+        <v>30</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1200000</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="0"/>
+        <v>600000</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E9" s="19">
+        <v>30</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="0"/>
+        <v>600000</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E10" s="19">
         <v>25</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="F10" s="6">
+        <v>800000</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="0"/>
+        <v>500000</v>
+      </c>
+      <c r="H10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E4" s="23">
-        <v>35</v>
-      </c>
-      <c r="F4" s="25">
-        <v>2100000</v>
-      </c>
-      <c r="G4" s="25">
-        <f>D4*E4</f>
-        <v>2100000</v>
-      </c>
-      <c r="H4" s="23" t="s">
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="27" t="s">
+      <c r="D11" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E11" s="19">
+        <v>20</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="28">
-        <v>60000</v>
-      </c>
-      <c r="E5" s="27">
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="29">
-        <v>0</v>
-      </c>
-      <c r="G5" s="29">
-        <f>D5*E5</f>
-        <v>2400000</v>
-      </c>
-      <c r="H5" s="30" t="s">
+      <c r="B12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="27"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E6" s="23">
-        <v>38</v>
-      </c>
-      <c r="F6" s="25">
-        <v>2086000</v>
-      </c>
-      <c r="G6" s="25">
-        <f>D6*E6</f>
-        <v>2280000</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="8" t="s">
+      <c r="D12" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E12" s="19">
+        <v>328</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6">
+        <v>26240000</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="28">
+        <f>SUM(G2:G12)</f>
+        <v>33400000</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="7"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="32"/>
+      <c r="B122" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E7" s="23">
+      <c r="C122" s="33"/>
+      <c r="D122" s="34"/>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B123" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="8">
-        <v>2000000</v>
-      </c>
-      <c r="G7" s="8">
-        <f>D7*E7</f>
-        <v>2700000</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E8" s="23">
-        <v>30</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1200000</v>
-      </c>
-      <c r="G8" s="8">
-        <f>D8*E8</f>
-        <v>1800000</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="23"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E9" s="23">
-        <v>30</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="G9" s="8">
-        <f>D9*E9</f>
-        <v>1800000</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="23"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E10" s="23">
-        <v>25</v>
-      </c>
-      <c r="F10" s="8">
-        <v>800000</v>
-      </c>
-      <c r="G10" s="8">
-        <f>D10*E10</f>
-        <v>1500000</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="24">
-        <v>60000</v>
-      </c>
-      <c r="E11" s="23">
-        <v>20</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="G11" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="23"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="33">
-        <f>G11+G10+G9+G8+G7+G6+G5+G4+G3+G2</f>
-        <v>19480000</v>
-      </c>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="37"/>
-      <c r="B120" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C120" s="38"/>
-      <c r="D120" s="39"/>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B121" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C121" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D121" s="40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B122" s="41" t="s">
+      <c r="C123" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C122" s="42">
+      <c r="D123" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B124" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C124" s="37">
         <v>55000</v>
       </c>
-      <c r="D122" s="43">
+      <c r="D124" s="38">
         <v>1100000</v>
       </c>
     </row>
-    <row r="123" ht="30" spans="1:4">
-      <c r="A123" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B123" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="C123" s="42">
+    <row r="125" ht="30" spans="1:4">
+      <c r="A125" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B125" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C125" s="37">
         <v>55000</v>
       </c>
-      <c r="D123" s="43">
+      <c r="D125" s="38">
         <v>1100000</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B124" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C124" s="42">
+    <row r="126" spans="1:4">
+      <c r="A126" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B126" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C126" s="37">
         <v>55000</v>
       </c>
-      <c r="D124" s="43">
+      <c r="D126" s="38">
         <v>550000</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
-      <c r="A125" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B125" s="44"/>
-      <c r="C125" s="44"/>
-      <c r="D125" s="45">
-        <f>D124+D123+D122</f>
+    <row r="127" spans="1:4">
+      <c r="A127" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B127" s="29"/>
+      <c r="C127" s="29"/>
+      <c r="D127" s="39">
+        <f>D126+D125+D124</f>
         <v>2750000</v>
       </c>
     </row>
@@ -2542,7 +2556,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2551,9 +2565,9 @@
     <col min="2" max="2" width="63.5714285714286" style="2" customWidth="1"/>
     <col min="3" max="3" width="15" style="3" customWidth="1"/>
     <col min="4" max="4" width="25.8571428571429" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.2857142857143" style="4" customWidth="1"/>
-    <col min="6" max="6" width="16.4285714285714" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.5714285714286" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.2857142857143" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.4285714285714" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.5714285714286" style="3" customWidth="1"/>
     <col min="8" max="8" width="16" style="2" customWidth="1"/>
     <col min="9" max="11" width="9" style="2"/>
     <col min="12" max="12" width="72.8571428571429" style="3" customWidth="1"/>
@@ -2562,189 +2576,189 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="L1"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="6">
         <v>25000</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="9">
         <f>D2*12</f>
         <v>300000</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="9">
         <f>D2*36</f>
         <v>900000</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="9">
         <f>D2*60</f>
         <v>1500000</v>
       </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="10"/>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="A3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="6">
         <v>61000</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <f>D3*12</f>
         <v>732000</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="9">
         <f>D3*36</f>
         <v>2196000</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="9">
         <f>D3*60</f>
         <v>3660000</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="10"/>
       <c r="L3"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="A4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="6">
         <v>46000</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <f>D4*12</f>
         <v>552000</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="9">
         <f>D4*36</f>
         <v>1656000</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="9">
         <f>D4*60</f>
         <v>2760000</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="A5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="6">
         <v>95000</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <f>D5*12</f>
         <v>1140000</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="9">
         <f>D5*36</f>
         <v>3420000</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="9">
         <f>D5*60</f>
         <v>5700000</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="A6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="6">
         <v>33874</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <f>D6*12</f>
         <v>406488</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="9">
         <f>D6*36</f>
         <v>1219464</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="9">
         <f>D6*60</f>
         <v>2032440</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16">
+      <c r="A7" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12">
         <f>E6+E5+E4+E3+E2</f>
         <v>3130488</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <f>F6+F5+F4+F3+F2</f>
         <v>9391464</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="12">
         <f>G6+G5+G4+G3+G2</f>
         <v>15652440</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="12" spans="2:4">
       <c r="B12"/>
@@ -2762,7 +2776,7 @@
       <c r="D14"/>
     </row>
     <row r="15" spans="2:2">
-      <c r="B15" s="9"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="18" spans="2:4">
       <c r="B18"/>
@@ -2863,28 +2877,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>